<commit_message>
Finished QAQC of bacteria loads, setting up data pipeline, and adding configs. Next just need to go through the BMPs.
</commit_message>
<xml_diff>
--- a/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
+++ b/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcamp\Documents\GitHub\TDEC_BacteriaModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95844CC3-5F95-4EB3-8626-94AA592914E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637695DD-CD81-451D-9064-A2764D650543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
   </bookViews>
   <sheets>
     <sheet name="Bacteria_BMP_Descriptions" sheetId="4" r:id="rId1"/>
@@ -49,6 +49,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={D9D24254-64AC-47FD-9814-97BB1B80E5E7}</author>
+    <author>tc={02CA1D5C-9503-4646-A6D1-80366CA7DF7A}</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0" shapeId="0" xr:uid="{D9D24254-64AC-47FD-9814-97BB1B80E5E7}">
@@ -59,6 +60,18 @@
     UPDATE THE DISCOUNT RATE</t>
       </text>
     </comment>
+    <comment ref="E9" authorId="1" shapeId="0" xr:uid="{02CA1D5C-9503-4646-A6D1-80366CA7DF7A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    fraction treated will vary at scale as the number of systems depends on HUC12 or NHDplus catchment
+Reply:
+    Could have the user supply?
+Reply:
+    Not considering proximity to waterway anymore</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -439,43 +452,6 @@
 filters have less runoff reduction capability. The removal rate and runoff redcuction coeffiecients used for bacteria reduction calculations are averages of many potential ST BMPs.</t>
   </si>
   <si>
-    <t>1) Calculate volume of water converted to runoff for the Drainage Area (DA) of the BMP
-        -- Design Rainfall Capture is the runoff depth captured per impervious acre. This is set to a defualt of 1 inch, but can vary from 0.05 to 2.5 inches depending on the BMP.
-        -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
-2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS). 
-        -- WQv BMP / WQv Watershed
-3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
-        -- Discount Rate = 1.2 * 0.9 = 1.08
-4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
-        -- Runoff Reduction = 0.36
-        -- Unreduced Runoff = 1 - 0.36 = 0.64
-4) Calculate the Total Removal Rate (Reduced Runoff + (Unreduced Runoff * Removal Rate)). This is the total amount removed by the BMP by reducing and treating runoff.
-        -- Removal Rate = 0.32
-        -- Total Removal Rate = 0.36 + (0.64 * 0.32) = 0.565
-5) Calculate the Final Reduction.
-        -- Reduction = WS Urban Load * Capture Proportion * Discount Rate * Total Removal Rate</t>
-  </si>
-  <si>
-    <t>1) Calculate volume of water converted to runoff for the Drainage Area (DA) of the BMP
-        -- Design Rainfall Capture is the runoff depth captured per impervious acre. This is set to a defualt of 1 inch, but can vary from 0.05 to 2.5 inches depending on the BMP.
-        -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
-2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS).
-        -- WQv BMP / WQv Watershed
-3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
-        -- Discount Rate = 1.2 * 0.9 = 1.08
-4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
-        -- Runoff Reduction = 0.15
-        -- Unreduced Runoff = 1 - 0.15 = 0.85
-4) Calculate the Total Removal Rate (Runoff Reduction + (Unreduced Runoff * Removal Rate)). This is the total amount removed by the BMP by reducing and treating runoff.
-        -- Removal Rate = 0.41
-        -- Total Removal Rate = 0.15 + (0.85 * 0.41) = 0.499
-5) Calculate the Final Reduction.
-        -- Reduction = WS Urban Load * Capture Proportion * Discount Rate * Total Removal Rate</t>
-  </si>
-  <si>
-    <t>Impervious Area, Whether the Conversion is to Forested or Pervious</t>
-  </si>
-  <si>
     <t>Land Use Areas</t>
   </si>
   <si>
@@ -519,20 +495,11 @@
   </si>
   <si>
     <t>Refers to the planting of trees on previously non-forested land. Load reduction differs depending on the land cover that was replaced by the forested cover.</t>
-  </si>
-  <si>
-    <t>1) Get Watershed Impervious Load per acre (bn MPN / acre) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
-2) Find the Loading Rate Reduction per acre for impervious surface converstion (e.g. Impervious Land Rate - Pervious/Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
-3) Calculate the final Reduction by multiplying the Impervious area treated by the loading rate reduction.
-        -- Reduction = Impervious Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
   </si>
   <si>
     <t>1) Find the Loading Rate Reduction per acre (e.g. Open Developed Land Rate - Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
 2) Multiply the Loading Rate Reduction by the Area Converted to get the bacteria reduction.
         -- Reduction = Converted Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
-  </si>
-  <si>
-    <t>Land Cover Acres Converted to Forest, Land Cover Class Converted</t>
   </si>
   <si>
     <t>1) User inputs the fraction of the HUC12 or NHDplus Catchment population that is informed by pet waste education.
@@ -711,20 +678,6 @@
         -- Reduction = Septic Reduction - Treatment Plant Load</t>
   </si>
   <si>
-    <t>1) Get annual Watershed Urban Load (bn MPN) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
-2) Calculate the Treatability of the watershed (Drainage Area / Watershed Area). This is a by-area re-allocation of the watershed bacteria load to the practice area.
-3) Calculate Total Removal Rate.
-        -- Runoff Reduction = 0.75
-        -- Removal Rate = 0.42
-        -- Total Removal Rate = Runoff Reduction + ((1 - Runoff Reduction) * Removal Rate) = 0.75 + ((1 - 0.75) * 0.42) = 0.855
-4) Get Discount rate for the Design (0.8) and Maintenance of this BMP (0.5).
-        -- Discount Rate = 0.8 * 0.5 = 0.4
-        -- Design Discount = Factor applied based on the adequacy of existing design standards, and whether these standards exists and if they are legally binding.
-        -- Maintenance Discount = Factor based on the type of maintenance conducted on treatment practices, and whether these standards exists and how well they are enforced.
-4) Multiply together values of steps 1 - 4 to get the total Reduction.
-        -- Reduction = Watershed Urban Load (bn MPN) * ( Drainage Area / Watershed Area ) * Total Removal Rate * Discount Rate</t>
-  </si>
-  <si>
     <t>1) Septic Pumping and Denitrification reduces bacterial load by changing the failure rate associated with septic systems.
 2) Calculate the fraction of Unsewered Dwelling Units that are undergoing treatment using EITHER the Fraction Willing to Change Behavoir and Awareness OR the given Number of Systems Treated.
         -- Fraction Treated = Fraction Willing to Change Behavior * Awareness of Message
@@ -738,6 +691,67 @@
                                                                   + (Delivery Ratio Adjacent to Waterway (1.00) * % of Septics near Waterway * Adjacent to Waterway Bacteria Decay (13.0%))
                                                 )</t>
   </si>
+  <si>
+    <t>1) Get annual Watershed Urban Load (bn MPN) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
+2) Calculate the Treatability of the watershed (Drainage Area / Watershed Area). This is a by-area re-allocation of the watershed bacteria load to the practice area.
+3) Calculate Total Removal Rate.
+        -- Runoff Reduction = 0.75
+        -- Removal Rate = 0.42
+        -- Total Removal Rate = Runoff Reduction + ((1 - Runoff Reduction) * Removal Rate) = 0.75 + ((1 - 0.75) * 0.42) = 0.855
+4) Get Discount rate for the Design (0.8) and Maintenance of this BMP (0.5).
+        -- Discount Rate = 0.6 * 0.5 = 0.3
+        -- Design Discount = Factor applied based on the adequacy of existing design standards, and whether these standards exists and if they are legally binding.
+        -- Maintenance Discount = Factor based on the type of maintenance conducted on treatment practices, and whether these standards exists and how well they are enforced.
+4) Multiply together values of steps 1 - 4 to get the total Reduction.
+        -- Reduction = Watershed Urban Load (bn MPN) * ( Drainage Area / Watershed Area ) * Total Removal Rate * Discount Rate</t>
+  </si>
+  <si>
+    <t>1) Calculate volume of water converted to runoff for the Drainage Area (DA) of the BMP
+        -- Design Rainfall Capture is the runoff depth captured per impervious acre. This is set to a defualt of 1 inch, but can vary from 0.05 to 2.5 inches depending on the BMP.
+        -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
+2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS). 
+        -- WQv BMP / WQv Watershed
+3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
+        -- Discount Rate = 1.0 * 0.9 = 0.9
+4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
+        -- Runoff Reduction = 0.36
+        -- Unreduced Runoff = 1 - 0.36 = 0.64
+4) Calculate the Total Removal Rate (Reduced Runoff + (Unreduced Runoff * Removal Rate)). This is the total amount removed by the BMP by reducing and treating runoff.
+        -- Removal Rate = 0.32
+        -- Total Removal Rate = 0.36 + (0.64 * 0.32) = 0.565
+5) Calculate the Final Reduction.
+        -- Reduction = WS Urban Load * Capture Proportion * Discount Rate * Total Removal Rate</t>
+  </si>
+  <si>
+    <t>1) Calculate volume of water converted to runoff for the Drainage Area (DA) of the BMP
+        -- Design Rainfall Capture is the runoff depth captured per impervious acre. This is set to a defualt of 1 inch, but can vary from 0.05 to 2.5 inches depending on the BMP.
+        -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
+2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS).
+        -- WQv BMP / WQv Watershed
+3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
+        -- Discount Rate = 1.0 * 0.9 = 0.9
+4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
+        -- Runoff Reduction = 0.15
+        -- Unreduced Runoff = 1 - 0.15 = 0.85
+4) Calculate the Total Removal Rate (Runoff Reduction + (Unreduced Runoff * Removal Rate)). This is the total amount removed by the BMP by reducing and treating runoff.
+        -- Removal Rate = 0.41
+        -- Total Removal Rate = 0.15 + (0.85 * 0.41) = 0.499
+5) Calculate the Final Reduction.
+        -- Reduction = WS Urban Load * Capture Proportion * Discount Rate * Total Removal Rate</t>
+  </si>
+  <si>
+    <t>Land Cover Acres Converted to Forest, Land Cover Class Converted (Ag or Urban)</t>
+  </si>
+  <si>
+    <t>Assumes that the impervious area is converted to natural cover.
+1) Get Watershed Impervious Load per acre (bn MPN / acre) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
+2) Find the Loading Rate Reduction per acre for impervious surface converstion (e.g. Impervious Land Rate - Pervious/Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
+3) Calculate the final Reduction by multiplying the Impervious area treated by the loading rate reduction.
+        -- Reduction = Impervious Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
+  </si>
+  <si>
+    <t>Impervious Area (acres)</t>
+  </si>
 </sst>
 </file>
 
@@ -747,7 +761,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -806,6 +820,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1360,23 +1380,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1795,6 +1815,15 @@
   <threadedComment ref="E5" dT="2021-03-29T13:14:53.45" personId="{44B9086C-A423-4903-B9E8-02436727975F}" id="{D9D24254-64AC-47FD-9814-97BB1B80E5E7}">
     <text>UPDATE THE DISCOUNT RATE</text>
   </threadedComment>
+  <threadedComment ref="E9" dT="2021-06-21T00:42:46.48" personId="{44B9086C-A423-4903-B9E8-02436727975F}" id="{02CA1D5C-9503-4646-A6D1-80366CA7DF7A}">
+    <text>fraction treated will vary at scale as the number of systems depends on HUC12 or NHDplus catchment</text>
+  </threadedComment>
+  <threadedComment ref="E9" dT="2021-06-21T00:43:30.11" personId="{44B9086C-A423-4903-B9E8-02436727975F}" id="{C89C1047-B8F0-49EE-B686-67285727E3EF}" parentId="{02CA1D5C-9503-4646-A6D1-80366CA7DF7A}">
+    <text>Could have the user supply?</text>
+  </threadedComment>
+  <threadedComment ref="E9" dT="2021-06-21T00:48:56.26" personId="{44B9086C-A423-4903-B9E8-02436727975F}" id="{88B06301-FBB6-4073-8E31-218FD37258F6}" parentId="{02CA1D5C-9503-4646-A6D1-80366CA7DF7A}">
+    <text>Not considering proximity to waterway anymore</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1854,14 +1883,14 @@
       <c r="N3" s="38"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="79">
+      <c r="B4" s="83">
         <v>12</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="79" t="s">
         <v>74</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>90</v>
@@ -1877,8 +1906,8 @@
       <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="79"/>
-      <c r="C5" s="81"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="85"/>
       <c r="E5" s="39" t="s">
         <v>91</v>
@@ -1894,8 +1923,8 @@
       <c r="N5" s="38"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="79"/>
-      <c r="C6" s="81"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="85"/>
       <c r="E6" s="39" t="s">
         <v>92</v>
@@ -1911,8 +1940,8 @@
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
-      <c r="C7" s="81"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="85"/>
       <c r="E7" s="39" t="s">
         <v>112</v>
@@ -1928,8 +1957,8 @@
       <c r="N7" s="38"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="79"/>
-      <c r="C8" s="81"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="85"/>
       <c r="E8" s="39" t="s">
         <v>93</v>
@@ -1945,8 +1974,8 @@
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="86"/>
       <c r="E9" s="49" t="s">
         <v>94</v>
@@ -1962,10 +1991,10 @@
       <c r="N9" s="38"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="79">
+      <c r="B10" s="83">
         <v>17</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="79" t="s">
         <v>81</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -1985,61 +2014,61 @@
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="79"/>
-      <c r="C11" s="81"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="85"/>
       <c r="E11" s="40" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="79"/>
-      <c r="C12" s="81"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="85"/>
       <c r="E12" s="40" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="79"/>
-      <c r="C13" s="81"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="85"/>
       <c r="E13" s="40" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="79"/>
-      <c r="C14" s="81"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="85"/>
       <c r="E14" s="40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="79"/>
-      <c r="C15" s="81"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="85"/>
       <c r="E15" s="40" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="80"/>
-      <c r="C16" s="83"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="86"/>
       <c r="E16" s="50" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="79">
+      <c r="B17" s="83">
         <v>18</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="81" t="s">
         <v>122</v>
       </c>
       <c r="E17" s="40" t="s">
@@ -2047,25 +2076,25 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="79"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="40" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="79"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="82"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="40" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="80"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="84"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="82"/>
       <c r="E20" s="50" t="s">
         <v>97</v>
       </c>
@@ -2083,13 +2112,13 @@
       <c r="E21" s="50"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="79">
+      <c r="B22" s="83">
         <v>20</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="81" t="s">
         <v>119</v>
       </c>
       <c r="E22" s="40" t="s">
@@ -2097,37 +2126,37 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="79"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="82"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="80"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="82"/>
       <c r="E24" s="50" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="79">
+      <c r="B25" s="83">
         <v>21</v>
       </c>
-      <c r="C25" s="81" t="s">
+      <c r="C25" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="40" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="80"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="82"/>
       <c r="E26" s="50" t="s">
         <v>109</v>
       </c>
@@ -2145,13 +2174,13 @@
       <c r="E27" s="50"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="79">
+      <c r="B28" s="83">
         <v>24</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="82" t="s">
+      <c r="D28" s="81" t="s">
         <v>120</v>
       </c>
       <c r="E28" s="40" t="s">
@@ -2159,9 +2188,9 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="79"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="82"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="40" t="s">
         <v>111</v>
       </c>
@@ -2192,6 +2221,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="B4:B9"/>
@@ -2204,12 +2239,6 @@
     <mergeCell ref="D10:D16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2219,15 +2248,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA82E1C4-00FB-4592-BD49-209EA9DB00EE}">
   <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
     <col min="5" max="5" width="177.42578125" customWidth="1"/>
   </cols>
@@ -2258,7 +2287,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -2269,10 +2298,10 @@
         <v>74</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="225" x14ac:dyDescent="0.25">
@@ -2286,7 +2315,7 @@
         <v>84</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="F5" s="52"/>
     </row>
@@ -2301,36 +2330,36 @@
         <v>84</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="F6" s="52"/>
     </row>
-    <row r="7" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="210" x14ac:dyDescent="0.25">
@@ -2341,10 +2370,10 @@
         <v>77</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="180" x14ac:dyDescent="0.25">
@@ -2355,13 +2384,13 @@
         <v>78</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>24</v>
       </c>
@@ -2369,10 +2398,10 @@
         <v>79</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="75" x14ac:dyDescent="0.25">
@@ -2386,7 +2415,7 @@
         <v>86</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2397,10 +2426,10 @@
         <v>116</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E13" s="78" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2408,9 +2437,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="77" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2478,13 +2507,13 @@
     <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B4" s="54"/>
       <c r="C4" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F4" s="23"/>
     </row>
@@ -2495,7 +2524,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>16</v>
@@ -2508,7 +2537,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>18</v>
@@ -2521,7 +2550,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F7" s="23"/>
     </row>
@@ -2529,10 +2558,10 @@
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F8" s="23"/>
     </row>
@@ -2543,7 +2572,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F9" s="26"/>
     </row>
@@ -2568,10 +2597,10 @@
       <c r="B11" s="54"/>
       <c r="C11" s="55"/>
       <c r="D11" s="55" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F11" s="56"/>
     </row>
@@ -2584,7 +2613,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F12" s="29"/>
     </row>
@@ -2634,7 +2663,7 @@
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F16" s="23"/>
     </row>
@@ -2885,13 +2914,13 @@
         <v>70</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E39" s="57" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F39" s="58"/>
     </row>
@@ -2915,7 +2944,7 @@
     </row>
     <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="68" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="70"/>
@@ -2924,10 +2953,10 @@
     </row>
     <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="61" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D43" s="62"/>
       <c r="E43"/>
@@ -2942,10 +2971,10 @@
     </row>
     <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D45" s="62"/>
       <c r="E45"/>
@@ -2957,17 +2986,17 @@
         <v>0.9</v>
       </c>
       <c r="D46" s="72" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
     </row>
     <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="61" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D47" s="62"/>
       <c r="E47"/>
@@ -2979,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="62" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E48"/>
       <c r="F48"/>
@@ -2990,7 +3019,7 @@
         <v>0.8</v>
       </c>
       <c r="D49" s="65" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E49"/>
       <c r="F49"/>
@@ -3001,17 +3030,17 @@
         <v>0.6</v>
       </c>
       <c r="D50" s="74" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E50"/>
       <c r="F50"/>
     </row>
     <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="61" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D51" s="62"/>
       <c r="E51"/>
@@ -3023,7 +3052,7 @@
         <v>0.9</v>
       </c>
       <c r="D52" s="62" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E52"/>
       <c r="F52"/>
@@ -3034,7 +3063,7 @@
         <v>0.6</v>
       </c>
       <c r="D53" s="65" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
@@ -3045,14 +3074,14 @@
         <v>0.5</v>
       </c>
       <c r="D54" s="67" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
     </row>
     <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="76" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished with all BMPs for bacteria reduction.
</commit_message>
<xml_diff>
--- a/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
+++ b/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcamp\Documents\GitHub\TDEC_BacteriaModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637695DD-CD81-451D-9064-A2764D650543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C818FB-64A1-4636-912C-A8A58609CCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
   </bookViews>
   <sheets>
     <sheet name="Bacteria_BMP_Descriptions" sheetId="4" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>CALCULATION</t>
   </si>
   <si>
-    <t>Drainage Area, Impervious Area</t>
-  </si>
-  <si>
     <t>Linear Feet</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
   </si>
   <si>
     <t>INPUT FROM USER</t>
-  </si>
-  <si>
-    <t>Drainage Area, Impervious Area, Design Rainfall Capture of BMP</t>
   </si>
   <si>
     <t>Population is redistributed from block group to the HUC12 / NHDplus catchment scale using by area weighing, assuming population is eqally spread across block group.</t>
@@ -495,11 +489,6 @@
   </si>
   <si>
     <t>Refers to the planting of trees on previously non-forested land. Load reduction differs depending on the land cover that was replaced by the forested cover.</t>
-  </si>
-  <si>
-    <t>1) Find the Loading Rate Reduction per acre (e.g. Open Developed Land Rate - Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
-2) Multiply the Loading Rate Reduction by the Area Converted to get the bacteria reduction.
-        -- Reduction = Converted Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
   </si>
   <si>
     <t>1) User inputs the fraction of the HUC12 or NHDplus Catchment population that is informed by pet waste education.
@@ -664,20 +653,6 @@
     <t>(Fraction Willing to Change Behavior, Awareness of Message) OR (Number of Systems Treated)</t>
   </si>
   <si>
-    <t>1) Determine the amount of Untreated Sewage Delivered to Septic Systems for the HUC12 or NHDplus catchment from a lookup table containing baseline model ouputs.
-2) Calculate the ratio of Retired Septic Systems to the Number of Unsewered Dwelling Units, assuming that 46% of dwelling units are unsewered ( # of Dwelling Units * 0.46 ).
-        -- Retirement Ratio = Retired Septic Systems / Number of Unsewered Dwelling Units
-3) Calculate the Sewage Treated by multiplying the Sewage Delivered to Septic Systems by the Retirement Ratio.
-        -- Sewage Treated = Untreated Sewage * Retirement Ratio
-4) Calculate the Reduction as the loading the Sewage Treated would have contributed had it not been connected to the sewer system.
-        -- Septic Reduction = (Sewage Treated * Septic Failure Rate (20%) * Normal Delivery Ratio (0.5) * % of Septics not near Waterway * Normal Bacteria Decay (0.20%))
-                                                   + (Delivery Ratio Adjacent to Waterway (1.00) * % of Septics near Waterway * Adjacent to Waterway Bacteria Decay (13.0%))
-5) Need to consider the now additional Treatment Plant Load and subtract this from the estimated Septic Reduction. This is done using a Bacteria Log Reduction Constant (1.0).
-        -- Treatment Plant Load = Sewage Treated * 10^( - Bacteria Log Reduction Constant)
-6) Calculate the final Reduction.
-        -- Reduction = Septic Reduction - Treatment Plant Load</t>
-  </si>
-  <si>
     <t>1) Septic Pumping and Denitrification reduces bacterial load by changing the failure rate associated with septic systems.
 2) Calculate the fraction of Unsewered Dwelling Units that are undergoing treatment using EITHER the Fraction Willing to Change Behavoir and Awareness OR the given Number of Systems Treated.
         -- Fraction Treated = Fraction Willing to Change Behavior * Awareness of Message
@@ -706,12 +681,22 @@
         -- Reduction = Watershed Urban Load (bn MPN) * ( Drainage Area / Watershed Area ) * Total Removal Rate * Discount Rate</t>
   </si>
   <si>
+    <t>Assumes that the impervious area is converted to natural cover.
+1) Get Watershed Impervious Load per acre (bn MPN / acre) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
+2) Find the Loading Rate Reduction per acre for impervious surface converstion (e.g. Impervious Land Rate - Pervious/Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
+3) Calculate the final Reduction by multiplying the Impervious area treated by the loading rate reduction.
+        -- Reduction = Impervious Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
+  </si>
+  <si>
+    <t>Drainage Area</t>
+  </si>
+  <si>
     <t>1) Calculate volume of water converted to runoff for the Drainage Area (DA) of the BMP
         -- Design Rainfall Capture is the runoff depth captured per impervious acre. This is set to a defualt of 1 inch, but can vary from 0.05 to 2.5 inches depending on the BMP.
         -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
 2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS). 
         -- WQv BMP / WQv Watershed
-3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
+3) Get Discount rate for the Design (1.0) and Maintenance of this BMP (0.9).
         -- Discount Rate = 1.0 * 0.9 = 0.9
 4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
         -- Runoff Reduction = 0.36
@@ -728,7 +713,7 @@
         -- WQv BMP = Design Rainfall Capture * (IA * Impervious Runoff Coeff + (DA - IA) * Pervious Runoff Coeff)
 2) Caclculate Capture Proportion for the drainage area of the BMP compared to the Watershed (WS).
         -- WQv BMP / WQv Watershed
-3) Get Discount rate for the Design (1.2) and Maintenance of this BMP (0.9).
+3) Get Discount rate for the Design (1.0) and Maintenance of this BMP (0.9).
         -- Discount Rate = 1.0 * 0.9 = 0.9
 4) Calculate Unreduced Runoff (1 - Runoff Reduction). This is the amount of runoff not treated by the BMP.
         -- Runoff Reduction = 0.15
@@ -740,17 +725,32 @@
         -- Reduction = WS Urban Load * Capture Proportion * Discount Rate * Total Removal Rate</t>
   </si>
   <si>
-    <t>Land Cover Acres Converted to Forest, Land Cover Class Converted (Ag or Urban)</t>
-  </si>
-  <si>
-    <t>Assumes that the impervious area is converted to natural cover.
-1) Get Watershed Impervious Load per acre (bn MPN / acre) for the HUC12 or NHDplus Catchment for the BMP from a lookup table containing baseline model outputs.
-2) Find the Loading Rate Reduction per acre for impervious surface converstion (e.g. Impervious Land Rate - Pervious/Forested Land Rate) for the HUC12 or NHDplus Catchment for the BMP.
-3) Calculate the final Reduction by multiplying the Impervious area treated by the loading rate reduction.
-        -- Reduction = Impervious Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
-  </si>
-  <si>
-    <t>Impervious Area (acres)</t>
+    <t>Drainage Area, Percent Impervious, Design Rainfall Capture of BMP</t>
+  </si>
+  <si>
+    <t>1) Determine the amount of Untreated Sewage Delivered to Septic Systems for the HUC12 or NHDplus catchment from a lookup table containing baseline model ouputs.
+2) Calculate the ratio of Retired Septic Systems to the Number of Unsewered Dwelling Units, assuming that 21% of dwelling units are unsewered ( # of Dwelling Units * 0.21 ).
+        -- Retirement Ratio = Retired Septic Systems / Number of Unsewered Dwelling Units
+3) Calculate the Sewage Treated by multiplying the Sewage Delivered to Septic Systems by the Retirement Ratio.
+        -- Sewage Treated = Untreated Sewage * Retirement Ratio
+4) Calculate the Reduction as the loading the Sewage Treated would have contributed had it not been connected to the sewer system.
+        -- Septic Reduction = (Sewage Treated * Septic Failure Rate (20%) * Normal Delivery Ratio (0.5) * % of Septics not near Waterway * Normal Bacteria Decay (0.20%))
+                                                   + (Delivery Ratio Adjacent to Waterway (1.00) * % of Septics near Waterway * Adjacent to Waterway Bacteria Decay (13.0%))
+5) Need to consider the now additional Treatment Plant Load and subtract this from the estimated Septic Reduction. This is done using a Bacteria Log Reduction Constant (1.0).
+        -- Treatment Plant Load = Septic Reduction * 10^( - Bacteria Log Reduction Constant)
+6) Calculate the final Reduction.
+        -- Reduction = Septic Reduction - Treatment Plant Load</t>
+  </si>
+  <si>
+    <t>Land Cover Acres Converted to Natural, Land Cover Class Converted (Ag or Urban)</t>
+  </si>
+  <si>
+    <t>1) Find the Loading Rate Reduction per acre (e.g. Urban or Ag Land Loading Rate - Forested/Natural Land Loading Rate) for the HUC12 or NHDplus Catchment for the BMP.
+2) Multiply the Loading Rate Reduction by the Area Converted to get the bacteria reduction.
+        -- Reduction = Converted Area (acres) * Loading Rate Reduction (bn MPN / acre)</t>
+  </si>
+  <si>
+    <t>Area (acres), Percent Impervious</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,12 +820,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1380,23 +1374,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1853,10 +1847,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="45" x14ac:dyDescent="0.25">
@@ -1864,13 +1858,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
@@ -1883,17 +1877,17 @@
       <c r="N3" s="38"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="83">
+      <c r="B4" s="79">
         <v>12</v>
       </c>
-      <c r="C4" s="79" t="s">
-        <v>74</v>
+      <c r="C4" s="81" t="s">
+        <v>73</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -1906,11 +1900,11 @@
       <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="85"/>
       <c r="E5" s="39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -1923,11 +1917,11 @@
       <c r="N5" s="38"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="83"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="85"/>
       <c r="E6" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -1940,11 +1934,11 @@
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="83"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="85"/>
       <c r="E7" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -1957,11 +1951,11 @@
       <c r="N7" s="38"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="83"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="85"/>
       <c r="E8" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -1974,11 +1968,11 @@
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="84"/>
-      <c r="C9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="86"/>
       <c r="E9" s="49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
@@ -1991,17 +1985,17 @@
       <c r="N9" s="38"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="83">
+      <c r="B10" s="79">
         <v>17</v>
       </c>
-      <c r="C10" s="79" t="s">
-        <v>81</v>
+      <c r="C10" s="81" t="s">
+        <v>80</v>
       </c>
       <c r="D10" s="85" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
@@ -2014,89 +2008,89 @@
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="85"/>
       <c r="E11" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="85"/>
       <c r="E12" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="83"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="81"/>
       <c r="D13" s="85"/>
       <c r="E13" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="83"/>
-      <c r="C14" s="79"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="85"/>
       <c r="E14" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="83"/>
-      <c r="C15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="85"/>
       <c r="E15" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="84"/>
-      <c r="C16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="86"/>
       <c r="E16" s="50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="83">
+      <c r="B17" s="79">
         <v>18</v>
       </c>
-      <c r="C17" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="81" t="s">
-        <v>122</v>
+      <c r="C17" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>120</v>
       </c>
       <c r="E17" s="40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="79"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="83"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="40" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="83"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="82"/>
       <c r="E19" s="40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="84"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="82"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -2104,61 +2098,61 @@
         <v>19</v>
       </c>
       <c r="C21" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="50"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="79">
+        <v>20</v>
+      </c>
+      <c r="C22" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="50"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="83">
-        <v>20</v>
-      </c>
-      <c r="C22" s="79" t="s">
+      <c r="D22" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="79"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="80"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="79">
+        <v>21</v>
+      </c>
+      <c r="C25" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="81" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="83"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="40" t="s">
+      <c r="D25" s="82"/>
+      <c r="E25" s="40" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="84"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="50" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="80"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="50" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="83">
-        <v>21</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="84"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="50" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -2166,33 +2160,33 @@
         <v>22</v>
       </c>
       <c r="C27" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="50"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="79">
+        <v>24</v>
+      </c>
+      <c r="C28" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="50"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="83">
-        <v>24</v>
-      </c>
-      <c r="C28" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="81" t="s">
-        <v>120</v>
+      <c r="D28" s="82" t="s">
+        <v>118</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="83"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="81"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
       <c r="E29" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -2200,10 +2194,10 @@
         <v>25</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E30" s="50"/>
     </row>
@@ -2212,21 +2206,15 @@
         <v>26</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E31" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="B4:B9"/>
@@ -2239,6 +2227,12 @@
     <mergeCell ref="D10:D16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2248,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA82E1C4-00FB-4592-BD49-209EA9DB00EE}">
   <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>2</v>
@@ -2281,13 +2275,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>3</v>
+        <v>166</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -2295,13 +2289,13 @@
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>171</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="225" x14ac:dyDescent="0.25">
@@ -2309,13 +2303,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F5" s="52"/>
     </row>
@@ -2324,13 +2318,13 @@
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F6" s="52"/>
     </row>
@@ -2339,13 +2333,13 @@
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2353,13 +2347,13 @@
         <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="210" x14ac:dyDescent="0.25">
@@ -2367,13 +2361,13 @@
         <v>21</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="180" x14ac:dyDescent="0.25">
@@ -2381,13 +2375,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="75" x14ac:dyDescent="0.25">
@@ -2395,13 +2389,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>173</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="75" x14ac:dyDescent="0.25">
@@ -2409,13 +2403,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2423,13 +2417,13 @@
         <v>26</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E13" s="78" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2439,7 +2433,7 @@
     </row>
     <row r="15" spans="2:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="C15" s="77" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2472,48 +2466,48 @@
     <row r="1" spans="2:6" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="20" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B4" s="54"/>
       <c r="C4" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F4" s="23"/>
     </row>
@@ -2521,36 +2515,36 @@
       <c r="B5" s="21"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" s="23"/>
     </row>
@@ -2558,10 +2552,10 @@
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F8" s="23"/>
     </row>
@@ -2569,76 +2563,76 @@
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F9" s="26"/>
     </row>
     <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="D10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="E10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="F10" s="28" t="s">
         <v>24</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="54"/>
       <c r="C11" s="55"/>
       <c r="D11" s="55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F11" s="56"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F12" s="29"/>
     </row>
     <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23"/>
@@ -2646,37 +2640,37 @@
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="21"/>
       <c r="C16" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F16" s="23"/>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
       <c r="C17" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="E17" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="F17" s="23"/>
     </row>
@@ -2689,13 +2683,13 @@
     </row>
     <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="D19" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="29"/>
@@ -2703,10 +2697,10 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
       <c r="C20" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="29"/>
@@ -2714,10 +2708,10 @@
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>45</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="29"/>
@@ -2725,10 +2719,10 @@
     <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
       <c r="C22" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="29"/>
@@ -2736,10 +2730,10 @@
     <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21"/>
       <c r="C23" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="29"/>
@@ -2753,13 +2747,13 @@
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="D25" s="31" t="s">
         <v>49</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>50</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="29"/>
@@ -2767,13 +2761,13 @@
     <row r="26" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21"/>
       <c r="C26" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="22" t="s">
         <v>51</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>52</v>
       </c>
       <c r="F26" s="29"/>
     </row>
@@ -2781,10 +2775,10 @@
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="29"/>
     </row>
@@ -2792,10 +2786,10 @@
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F28" s="29"/>
     </row>
@@ -2803,21 +2797,21 @@
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F29" s="29"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="21"/>
       <c r="C30" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" s="33"/>
     </row>
@@ -2825,10 +2819,10 @@
       <c r="B31" s="21"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>58</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>59</v>
       </c>
       <c r="F31" s="33"/>
     </row>
@@ -2837,20 +2831,20 @@
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
       <c r="E32" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="33"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
       <c r="C33" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>61</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="F33" s="33"/>
     </row>
@@ -2858,10 +2852,10 @@
       <c r="B34" s="21"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="32" t="s">
         <v>63</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="F34" s="33"/>
     </row>
@@ -2869,10 +2863,10 @@
       <c r="B35" s="21"/>
       <c r="C35" s="32"/>
       <c r="D35" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>65</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>66</v>
       </c>
       <c r="F35" s="33"/>
     </row>
@@ -2880,20 +2874,20 @@
       <c r="B36" s="21"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" s="33"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="21"/>
       <c r="C37" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="29"/>
@@ -2901,36 +2895,36 @@
     <row r="38" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="21"/>
       <c r="C38" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>69</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="29"/>
     </row>
     <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C39" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="57" t="s">
         <v>134</v>
-      </c>
-      <c r="D39" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="57" t="s">
-        <v>136</v>
       </c>
       <c r="F39" s="58"/>
     </row>
     <row r="40" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="59"/>
       <c r="C40" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="E40" s="34"/>
       <c r="F40" s="35"/>
@@ -2944,7 +2938,7 @@
     </row>
     <row r="42" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="68" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C42" s="69"/>
       <c r="D42" s="70"/>
@@ -2953,10 +2947,10 @@
     </row>
     <row r="43" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="61" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D43" s="62"/>
       <c r="E43"/>
@@ -2971,10 +2965,10 @@
     </row>
     <row r="45" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D45" s="62"/>
       <c r="E45"/>
@@ -2986,17 +2980,17 @@
         <v>0.9</v>
       </c>
       <c r="D46" s="72" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E46"/>
       <c r="F46"/>
     </row>
     <row r="47" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="61" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D47" s="62"/>
       <c r="E47"/>
@@ -3008,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="62" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E48"/>
       <c r="F48"/>
@@ -3019,7 +3013,7 @@
         <v>0.8</v>
       </c>
       <c r="D49" s="65" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E49"/>
       <c r="F49"/>
@@ -3030,17 +3024,17 @@
         <v>0.6</v>
       </c>
       <c r="D50" s="74" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E50"/>
       <c r="F50"/>
     </row>
     <row r="51" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="61" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D51" s="62"/>
       <c r="E51"/>
@@ -3052,7 +3046,7 @@
         <v>0.9</v>
       </c>
       <c r="D52" s="62" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E52"/>
       <c r="F52"/>
@@ -3063,7 +3057,7 @@
         <v>0.6</v>
       </c>
       <c r="D53" s="65" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E53"/>
       <c r="F53"/>
@@ -3074,14 +3068,14 @@
         <v>0.5</v>
       </c>
       <c r="D54" s="67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
     </row>
     <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="76" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding a non-DB version of the final outputs for base bacteria loads.
</commit_message>
<xml_diff>
--- a/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
+++ b/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcamp\Documents\GitHub\TDEC_BacteriaModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C818FB-64A1-4636-912C-A8A58609CCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769369D6-C8D3-417B-9CC7-512DD5877C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
   </bookViews>
@@ -1374,23 +1374,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1877,10 +1877,10 @@
       <c r="N3" s="38"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="79">
+      <c r="B4" s="83">
         <v>12</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="79" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="85" t="s">
@@ -1900,8 +1900,8 @@
       <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="79"/>
-      <c r="C5" s="81"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="85"/>
       <c r="E5" s="39" t="s">
         <v>89</v>
@@ -1917,8 +1917,8 @@
       <c r="N5" s="38"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="79"/>
-      <c r="C6" s="81"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="85"/>
       <c r="E6" s="39" t="s">
         <v>90</v>
@@ -1934,8 +1934,8 @@
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
-      <c r="C7" s="81"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="85"/>
       <c r="E7" s="39" t="s">
         <v>110</v>
@@ -1951,8 +1951,8 @@
       <c r="N7" s="38"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="79"/>
-      <c r="C8" s="81"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="85"/>
       <c r="E8" s="39" t="s">
         <v>91</v>
@@ -1968,8 +1968,8 @@
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="80"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="86"/>
       <c r="E9" s="49" t="s">
         <v>92</v>
@@ -1985,10 +1985,10 @@
       <c r="N9" s="38"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="79">
+      <c r="B10" s="83">
         <v>17</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="79" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -2008,61 +2008,61 @@
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="79"/>
-      <c r="C11" s="81"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="85"/>
       <c r="E11" s="40" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="79"/>
-      <c r="C12" s="81"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="85"/>
       <c r="E12" s="40" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="79"/>
-      <c r="C13" s="81"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="85"/>
       <c r="E13" s="40" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="79"/>
-      <c r="C14" s="81"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="85"/>
       <c r="E14" s="40" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="79"/>
-      <c r="C15" s="81"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="85"/>
       <c r="E15" s="40" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="80"/>
-      <c r="C16" s="83"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="86"/>
       <c r="E16" s="50" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="79">
+      <c r="B17" s="83">
         <v>18</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="81" t="s">
         <v>120</v>
       </c>
       <c r="E17" s="40" t="s">
@@ -2070,25 +2070,25 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="79"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="40" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="79"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="82"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="80"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="84"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="82"/>
       <c r="E20" s="50" t="s">
         <v>95</v>
       </c>
@@ -2106,13 +2106,13 @@
       <c r="E21" s="50"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="79">
+      <c r="B22" s="83">
         <v>20</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="81" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="40" t="s">
@@ -2120,37 +2120,37 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="79"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="82"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="40" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="80"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="82"/>
       <c r="E24" s="50" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="79">
+      <c r="B25" s="83">
         <v>21</v>
       </c>
-      <c r="C25" s="81" t="s">
+      <c r="C25" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="80"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="84"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="82"/>
       <c r="E26" s="50" t="s">
         <v>107</v>
       </c>
@@ -2168,13 +2168,13 @@
       <c r="E27" s="50"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="79">
+      <c r="B28" s="83">
         <v>24</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="82" t="s">
+      <c r="D28" s="81" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="40" t="s">
@@ -2182,9 +2182,9 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="79"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="82"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="40" t="s">
         <v>109</v>
       </c>
@@ -2215,6 +2215,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="B4:B9"/>
@@ -2227,12 +2233,6 @@
     <mergeCell ref="D10:D16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2242,7 +2242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA82E1C4-00FB-4592-BD49-209EA9DB00EE}">
   <dimension ref="B1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding in DB backups for the main model outputs.
</commit_message>
<xml_diff>
--- a/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
+++ b/DTAP_BacteriaBMPs_Desc_Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcamp\Documents\GitHub\TDEC_BacteriaModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769369D6-C8D3-417B-9CC7-512DD5877C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6759CBB9-97D5-4A4B-9FEB-FA46A1E2CC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B38986BF-9696-4238-B27D-AACFE491B87A}"/>
   </bookViews>
@@ -1374,23 +1374,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1877,10 +1877,10 @@
       <c r="N3" s="38"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="83">
+      <c r="B4" s="79">
         <v>12</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="81" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="85" t="s">
@@ -1900,8 +1900,8 @@
       <c r="N4" s="38"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
-      <c r="C5" s="79"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="85"/>
       <c r="E5" s="39" t="s">
         <v>89</v>
@@ -1917,8 +1917,8 @@
       <c r="N5" s="38"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="83"/>
-      <c r="C6" s="79"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="85"/>
       <c r="E6" s="39" t="s">
         <v>90</v>
@@ -1934,8 +1934,8 @@
       <c r="N6" s="38"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="83"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="85"/>
       <c r="E7" s="39" t="s">
         <v>110</v>
@@ -1951,8 +1951,8 @@
       <c r="N7" s="38"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="83"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="85"/>
       <c r="E8" s="39" t="s">
         <v>91</v>
@@ -1968,8 +1968,8 @@
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="84"/>
-      <c r="C9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="86"/>
       <c r="E9" s="49" t="s">
         <v>92</v>
@@ -1985,10 +1985,10 @@
       <c r="N9" s="38"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="83">
+      <c r="B10" s="79">
         <v>17</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="81" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -2008,61 +2008,61 @@
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="85"/>
       <c r="E11" s="40" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="85"/>
       <c r="E12" s="40" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="83"/>
-      <c r="C13" s="79"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="81"/>
       <c r="D13" s="85"/>
       <c r="E13" s="40" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="83"/>
-      <c r="C14" s="79"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="85"/>
       <c r="E14" s="40" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="83"/>
-      <c r="C15" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="85"/>
       <c r="E15" s="40" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="84"/>
-      <c r="C16" s="80"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="86"/>
       <c r="E16" s="50" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="83">
+      <c r="B17" s="79">
         <v>18</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="D17" s="82" t="s">
         <v>120</v>
       </c>
       <c r="E17" s="40" t="s">
@@ -2070,25 +2070,25 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="83"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="81"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
       <c r="E18" s="40" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="83"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="82"/>
       <c r="E19" s="40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="84"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="82"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="50" t="s">
         <v>95</v>
       </c>
@@ -2106,13 +2106,13 @@
       <c r="E21" s="50"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="83">
+      <c r="B22" s="79">
         <v>20</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="81" t="s">
+      <c r="D22" s="82" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="40" t="s">
@@ -2120,37 +2120,37 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="83"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="81"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="82"/>
       <c r="E23" s="40" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="84"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="82"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="50" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="83">
+      <c r="B25" s="79">
         <v>21</v>
       </c>
-      <c r="C25" s="79" t="s">
+      <c r="C25" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="81"/>
+      <c r="D25" s="82"/>
       <c r="E25" s="40" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="84"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="82"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="50" t="s">
         <v>107</v>
       </c>
@@ -2168,13 +2168,13 @@
       <c r="E27" s="50"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="83">
+      <c r="B28" s="79">
         <v>24</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="81" t="s">
+      <c r="D28" s="82" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="40" t="s">
@@ -2182,9 +2182,9 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="83"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="81"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
       <c r="E29" s="40" t="s">
         <v>109</v>
       </c>
@@ -2215,12 +2215,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="B4:B9"/>
@@ -2233,6 +2227,12 @@
     <mergeCell ref="D10:D16"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D17:D20"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>